<commit_message>
Updated list of inputs for plotting
</commit_message>
<xml_diff>
--- a/Data inputs for plotting.xlsx
+++ b/Data inputs for plotting.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheng\Documents\Jupyter Notebook\Tools for Analytics\Fall 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E9FA294-3455-4C64-9D96-D85E8673465E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FBBA4E-F492-4170-9CE1-A9A421576489}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="2" r:id="rId1"/>
-    <sheet name="Fed" sheetId="1" r:id="rId2"/>
-    <sheet name="Trade" sheetId="3" r:id="rId3"/>
+    <sheet name="Input List" sheetId="4" r:id="rId1"/>
+    <sheet name="General" sheetId="2" r:id="rId2"/>
+    <sheet name="Fed" sheetId="1" r:id="rId3"/>
+    <sheet name="Trade" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
   <si>
     <t>Input</t>
   </si>
@@ -66,9 +67,6 @@
     <t>2.a</t>
   </si>
   <si>
-    <t>industry of 30 US stocks</t>
-  </si>
-  <si>
     <t>energy, telecom, etc</t>
   </si>
   <si>
@@ -78,18 +76,12 @@
     <t>No. of each industry</t>
   </si>
   <si>
-    <t>event name</t>
-  </si>
-  <si>
     <t>raise rate to 0.25%-0.5%</t>
   </si>
   <si>
     <t>2.b</t>
   </si>
   <si>
-    <t>industry of 10 CN stocks</t>
-  </si>
-  <si>
     <t>Avg ab returns of 30 US stocks</t>
   </si>
   <si>
@@ -99,15 +91,9 @@
     <t>line</t>
   </si>
   <si>
-    <t>industry</t>
-  </si>
-  <si>
     <t>2.c</t>
   </si>
   <si>
-    <t>industry of 40 stocks</t>
-  </si>
-  <si>
     <t>Cumu ab return of each industry</t>
   </si>
   <si>
@@ -154,13 +140,106 @@
   </si>
   <si>
     <t>US/ENERGY</t>
+  </si>
+  <si>
+    <t>Trade event name</t>
+  </si>
+  <si>
+    <t>Fed event name</t>
+  </si>
+  <si>
+    <t>US industry</t>
+  </si>
+  <si>
+    <t>US + CN industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US industry </t>
+  </si>
+  <si>
+    <t>CN industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US + CN industry </t>
+  </si>
+  <si>
+    <t>Both event names</t>
+  </si>
+  <si>
+    <t>Fed</t>
+  </si>
+  <si>
+    <t>number of fed events</t>
+  </si>
+  <si>
+    <t>number of US industries</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>list of number (8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line </t>
+  </si>
+  <si>
+    <t>Avg ab returns of 30 US stocks per Fed event</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>CN Industry</t>
+  </si>
+  <si>
+    <t>number of Trade events</t>
+  </si>
+  <si>
+    <t>number of CN industries</t>
+  </si>
+  <si>
+    <t>number of stocks per CN industry</t>
+  </si>
+  <si>
+    <t>number of stocks per US industry</t>
+  </si>
+  <si>
+    <t>Country (U.S. &amp; CN) (2)</t>
+  </si>
+  <si>
+    <t>Avg ab returns of China stocks per trade event (24)</t>
+  </si>
+  <si>
+    <t>Avg ab returns of US stocks per trade event (24)</t>
+  </si>
+  <si>
+    <t>Avg cumu ab return of each industry (US + CN)</t>
+  </si>
+  <si>
+    <t>Cumu ab return of each US industry for Fed</t>
+  </si>
+  <si>
+    <t>Avg ab returns of each US indusrty for Fed</t>
+  </si>
+  <si>
+    <t>Avg cumu ab returns of China/US stock for Trade (2)</t>
+  </si>
+  <si>
+    <t>number of CN+US Industry</t>
+  </si>
+  <si>
+    <t>Avg ab returns of each indusrty per trade event (US + CN)</t>
+  </si>
+  <si>
+    <t>Avg cumu ab returns of China/US stock/each industry for Trade (num ind*2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -169,6 +248,36 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,6 +314,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,19 +632,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C0520F-217C-41CB-8AAC-934189CACB93}">
+  <dimension ref="A2:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -575,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -598,16 +837,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
@@ -618,19 +857,19 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>11</v>
@@ -641,19 +880,19 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>11</v>
@@ -671,7 +910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -679,7 +918,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,24 +971,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -757,49 +996,49 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>24</v>
+      <c r="I5" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -811,12 +1050,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499EA4A2-1E6F-4229-BE5B-0DA4563926F5}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -870,73 +1109,73 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,49 +1183,49 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -994,22 +1233,22 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>